<commit_message>
update result csv with corrected goldstandard link numbers
</commit_message>
<xml_diff>
--- a/results/CodeBERT.xlsx
+++ b/results/CodeBERT.xlsx
@@ -171,11 +171,11 @@
   </sheetPr>
   <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R16" activeCellId="0" sqref="R16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -191,15 +191,15 @@
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="1" t="n">
-        <v>7611</v>
+        <v>7610</v>
       </c>
       <c r="K1" s="2"/>
-      <c r="L1" s="1" t="n">
-        <v>1473</v>
+      <c r="L1" s="0" t="n">
+        <v>1295</v>
       </c>
       <c r="N1" s="2"/>
       <c r="O1" s="1" t="n">
-        <v>8268</v>
+        <v>8240</v>
       </c>
       <c r="Q1" s="2"/>
       <c r="T1" s="2"/>
@@ -369,15 +369,15 @@
       </c>
       <c r="T4" s="4" t="n">
         <f aca="false">(B4*$C1+E4*$F1+H4*$I1+K4*$L1+N4*$O1)/(SUM($C1,$F1,$I1,$L1,$O1))</f>
-        <v>0.278189850350654</v>
+        <v>0.279939112948274</v>
       </c>
       <c r="U4" s="4" t="n">
         <f aca="false">(C4*$C1+F4*$F1+I4*$I1+L4*$L1+O4*$O1)/(SUM($C1,$F1,$I1,$L1,$O1))</f>
-        <v>0.533857198078304</v>
+        <v>0.533847614791643</v>
       </c>
       <c r="V4" s="4" t="n">
         <f aca="false">(D4*$C1+G4*$F1+J4*$I1+M4*$L1+P4*$O1)/(SUM($C1,$F1,$I1,$L1,$O1))</f>
-        <v>0.353226572422552</v>
+        <v>0.355156965702156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>